<commit_message>
<feat> (reestrcutura del proyecto para la orquestación y pipeline feature): se realiza una corrección a la estructura del proyecto para la orquestación y se testea y prueba los primeros nodos del pipeline feature.
</commit_message>
<xml_diff>
--- a/data/01_raw/tag_dict_segmentacion.xlsx
+++ b/data/01_raw/tag_dict_segmentacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agomezj/Desktop/Data Science/Proyectos/proyecto_segmentacion/data/01_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AD1FBC-8067-CA40-848D-718A3D45F9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB84F7CC-9CE2-E645-8914-6BC44F4E02E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
   <si>
     <t>tag</t>
   </si>
@@ -235,9 +235,6 @@
     <t>canal_agrupacion</t>
   </si>
   <si>
-    <t>visitas_fds</t>
-  </si>
-  <si>
     <t>hora_visita</t>
   </si>
   <si>
@@ -250,16 +247,16 @@
     <t>pag_vistas_sesion</t>
   </si>
   <si>
-    <t>tasa_rebotes</t>
-  </si>
-  <si>
     <t>medio_trafico</t>
   </si>
   <si>
     <t>bool</t>
   </si>
   <si>
-    <t>s</t>
+    <t>tasa_visitas_fds</t>
+  </si>
+  <si>
+    <t>tasa_rebote</t>
   </si>
 </sst>
 </file>
@@ -285,16 +282,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -357,20 +357,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -601,441 +599,432 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="C5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="6" t="s">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="6" t="s">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="7" t="s">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="C13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="6" t="s">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="3"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="3"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="3"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="3"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="3"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="3"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="3"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="3"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="3"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="3"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E40" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>